<commit_message>
Envelope Breaking has been corrected
</commit_message>
<xml_diff>
--- a/wwwroot/75/ExtrasCalculation.xlsx
+++ b/wwwroot/75/ExtrasCalculation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>CenterCode</t>
   </si>
@@ -38,34 +38,61 @@
     <t>University Extra</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>AGS201</t>
-  </si>
-  <si>
-    <t>02-09-2025</t>
-  </si>
-  <si>
-    <t>09:00 AM to 12:00 PM</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>AS201</t>
-  </si>
-  <si>
-    <t>02:00 PM to 05:00 PM</t>
-  </si>
-  <si>
-    <t>AS213</t>
-  </si>
-  <si>
-    <t>BABED201</t>
-  </si>
-  <si>
-    <t>BED201</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>126305</t>
+  </si>
+  <si>
+    <t>07-04-2025</t>
+  </si>
+  <si>
+    <t>10:00 AM TO 01:00 PM</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>303001</t>
+  </si>
+  <si>
+    <t>08-04-2025</t>
+  </si>
+  <si>
+    <t>02:00 PM TO 05:00 PM</t>
+  </si>
+  <si>
+    <t>303002</t>
+  </si>
+  <si>
+    <t>09-04-2025</t>
+  </si>
+  <si>
+    <t>303015</t>
+  </si>
+  <si>
+    <t>17-04-2025</t>
+  </si>
+  <si>
+    <t>310021</t>
+  </si>
+  <si>
+    <t>311511</t>
+  </si>
+  <si>
+    <t>321015</t>
+  </si>
+  <si>
+    <t>321125</t>
+  </si>
+  <si>
+    <t>321165</t>
+  </si>
+  <si>
+    <t>321175</t>
+  </si>
+  <si>
+    <t>321235</t>
   </si>
 </sst>
 </file>
@@ -117,7 +144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr ">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -125,9 +152,9 @@
   <cols>
     <col min="1" max="1" width="16.09404182434082" customWidth="1"/>
     <col min="2" max="2" width="9.218536376953125" customWidth="1"/>
-    <col min="3" max="3" width="12.01124095916748" customWidth="1"/>
+    <col min="3" max="3" width="9.162454605102539" customWidth="1"/>
     <col min="4" max="4" width="13.382554054260254" customWidth="1"/>
-    <col min="5" max="5" width="22.885726928710938" customWidth="1"/>
+    <col min="5" max="5" width="23.803110122680664" customWidth="1"/>
     <col min="6" max="6" width="11.987889289855957" customWidth="1"/>
     <col min="7" max="7" width="12.143038749694824" customWidth="1"/>
   </cols>
@@ -189,10 +216,10 @@
         <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>12</v>
@@ -209,13 +236,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>12</v>
@@ -232,13 +259,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>12</v>
@@ -255,7 +282,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
@@ -278,7 +305,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
@@ -301,13 +328,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
@@ -324,13 +351,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>12</v>
@@ -347,10 +374,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>11</v>
@@ -370,10 +397,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>11</v>
@@ -382,6 +409,29 @@
         <v>12</v>
       </c>
       <c r="G11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>